<commit_message>
Added forgotten Level column
</commit_message>
<xml_diff>
--- a/bangarang/OLR/standard_input_bangarang.xlsx
+++ b/bangarang/OLR/standard_input_bangarang.xlsx
@@ -26,7 +26,7 @@
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="654">
   <si>
     <t>text</t>
   </si>
@@ -2148,6 +2148,9 @@
   </si>
   <si>
     <t>The 'bangarang' package is also available on GitHub - &lt;a href="https://github.com/ericmkeen/bangarang"&gt;GitHub link&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Component</t>
   </si>
 </sst>
 </file>
@@ -3190,191 +3193,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21" style="3" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22" style="3" customWidth="1"/>
-    <col min="6" max="6" width="51.5703125" style="3" customWidth="1"/>
-    <col min="7" max="9" width="45.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="45.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="32.28515625" style="3" customWidth="1"/>
-    <col min="14" max="17" width="57.28515625" style="3" customWidth="1"/>
-    <col min="18" max="20" width="42.85546875" style="3" customWidth="1"/>
-    <col min="21" max="21" width="84.28515625" style="3" customWidth="1"/>
+    <col min="1" max="2" width="21" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="22" style="3" customWidth="1"/>
+    <col min="7" max="7" width="51.5703125" style="3" customWidth="1"/>
+    <col min="8" max="10" width="45.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="45.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="32.28515625" style="3" customWidth="1"/>
+    <col min="15" max="18" width="57.28515625" style="3" customWidth="1"/>
+    <col min="19" max="21" width="42.85546875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>337</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>646</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>470</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>466</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>488</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>620</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>627</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>506</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="R1" s="16" t="s">
         <v>628</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>454</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>509</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="U1" s="16" t="s">
         <v>459</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>631</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>635</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>635</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>636</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>640</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>630</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>651</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>630</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>650</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="E1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="F1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3386,43 +3401,43 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F1</xm:sqref>
+          <xm:sqref>G1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'CV values'!$D$2:$D$60</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E1048576</xm:sqref>
+          <xm:sqref>F3:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>J1</xm:sqref>
+          <xm:sqref>K1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>R1:T1</xm:sqref>
+          <xm:sqref>S1:U1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>U1</xm:sqref>
+          <xm:sqref>V1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$B$1:$B$233</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:I1</xm:sqref>
+          <xm:sqref>H1:J1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>N1:Q1</xm:sqref>
+          <xm:sqref>O1:R1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Changed unique ID, for some reason reporting duplicate object
</commit_message>
<xml_diff>
--- a/bangarang/OLR/standard_input_bangarang.xlsx
+++ b/bangarang/OLR/standard_input_bangarang.xlsx
@@ -2039,9 +2039,6 @@
     <t>Identifier:identifier</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
     <t>The Bangarang Project</t>
   </si>
   <si>
@@ -2151,6 +2148,9 @@
   </si>
   <si>
     <t>Component</t>
+  </si>
+  <si>
+    <t>1001</t>
   </si>
 </sst>
 </file>
@@ -3196,7 +3196,7 @@
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3225,7 +3225,7 @@
         <v>485</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>2</v>
@@ -3287,69 +3287,69 @@
     </row>
     <row r="2" spans="1:22" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>630</v>
+        <v>653</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>484</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="T2" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>641</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>644</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>645</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>630</v>
+        <v>653</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>402</v>
@@ -3358,24 +3358,24 @@
         <v>357</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>651</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>630</v>
+        <v>653</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>383</v>
@@ -3384,7 +3384,7 @@
         <v>357</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reworked OLR with new template to pass validation on staging
</commit_message>
<xml_diff>
--- a/bangarang/OLR/standard_input_bangarang.xlsx
+++ b/bangarang/OLR/standard_input_bangarang.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" tabRatio="359"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="7275" tabRatio="351"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -58,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -128,26 +128,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>COLLECTION RECORD ONLY</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="653">
   <si>
     <t>text</t>
   </si>
@@ -155,6 +141,9 @@
     <t>Title</t>
   </si>
   <si>
+    <t>File name</t>
+  </si>
+  <si>
     <t>File use</t>
   </si>
   <si>
@@ -2009,9 +1998,6 @@
     <t>Person:Painter</t>
   </si>
   <si>
-    <t>Brief description</t>
-  </si>
-  <si>
     <t>Subject:culturalContext</t>
   </si>
   <si>
@@ -2039,9 +2025,45 @@
     <t>Identifier:identifier</t>
   </si>
   <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>readme.pdf</t>
+  </si>
+  <si>
+    <t>Summary data</t>
+  </si>
+  <si>
+    <t>Readme</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>Kitimat Fjord System</t>
+  </si>
+  <si>
+    <t>This archive file contains all the data in the collection.</t>
+  </si>
+  <si>
+    <t>10001</t>
+  </si>
+  <si>
+    <t>public_data_archive.zip</t>
+  </si>
+  <si>
+    <t>data | still image</t>
+  </si>
+  <si>
     <t>The Bangarang Project</t>
   </si>
   <si>
+    <t>Keen, Eric M.</t>
+  </si>
+  <si>
+    <t>Picard, Chris R.</t>
+  </si>
+  <si>
     <t>May 2013 - September 2015</t>
   </si>
   <si>
@@ -2049,31 +2071,10 @@
   </si>
   <si>
     <t>2015-09-30</t>
-  </si>
-  <si>
-    <t>Keen, Eric M.</t>
-  </si>
-  <si>
-    <t>Picard, Chris R.</t>
-  </si>
-  <si>
-    <t>data | text</t>
-  </si>
-  <si>
-    <t>Kitimat Fjord System</t>
-  </si>
-  <si>
-    <t>Humpback whale | Gitga'at First Nation | Fin whale</t>
   </si>
   <si>
     <t>Public Data Collection of the "Bangarang Project", the dissertation project of Eric Keen at Scripps Institution of Oceanography. These data are used in multiple chapters of that dissertation as well as their corresponding peer-reviewed publications. More information about this research can be found at its website: &lt;a href="https://rvbangarang.org/"&gt;rvbangarang.org&lt;/a&gt;.
 Metadata were prepared by Eric Keen, &lt;a href="mailto:ekeen@ucsd.edu"&gt;ekeen@ucsd.edu&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>Data associated with the "Bangarang Project", Eric Keen's dissertation study on the foraging ecology of whales in the Kitimat Fjord System, British Columbia.</t>
-  </si>
-  <si>
-    <t>Bangarang Site @ https://rvbangarang.org/</t>
   </si>
   <si>
     <t>2013_x000D_
@@ -2112,6 +2113,9 @@
 Robert and Patricia Ayres</t>
   </si>
   <si>
+    <t>The 'bangarang' package is also available on GitHub - &lt;a href="https://github.com/ericmkeen/bangarang"&gt;GitHub link&lt;/a&gt;</t>
+  </si>
+  <si>
     <t>Keen, EM. (In Preparation) Habitat use strategies of sympatric rorqual whales within a fjord system: what does “critical habitat” mean for mobile marine predators? Doctoral Thesis. University of California: San Diego._x000D_
 _x000D_
 Keen, EM, et al. (In Review) From fjord to fin: dive energetics link ocean features to competitive dynamics in sympatric rorqual whales. PLOS ONE._x000D_
@@ -2126,31 +2130,10 @@
     <t>Megaptera novaeangliae | Balaenoptera physalus</t>
   </si>
   <si>
-    <t>File name</t>
-  </si>
-  <si>
-    <t>readme.pdf</t>
-  </si>
-  <si>
-    <t>public_data_archive.zip</t>
-  </si>
-  <si>
-    <t>Summary data</t>
-  </si>
-  <si>
-    <t>Readme</t>
-  </si>
-  <si>
-    <t>This archive file contains all the data in the collection.</t>
-  </si>
-  <si>
-    <t>The 'bangarang' package is also available on GitHub - &lt;a href="https://github.com/ericmkeen/bangarang"&gt;GitHub link&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Component</t>
-  </si>
-  <si>
-    <t>1001</t>
+    <t>Humpback whale | Gitga'at First Nation | Fin whale</t>
+  </si>
+  <si>
+    <t>Bangarang Site @ https://rvbangarang.org/</t>
   </si>
 </sst>
 </file>
@@ -2388,7 +2371,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2588,12 +2571,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2820,14 +2797,12 @@
     <xf numFmtId="49" fontId="16" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3196,195 +3171,194 @@
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21" style="3" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21" style="3" customWidth="1"/>
+    <col min="2" max="3" width="34.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="22" style="3" customWidth="1"/>
     <col min="7" max="7" width="51.5703125" style="3" customWidth="1"/>
     <col min="8" max="10" width="45.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="45.5703125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="32.28515625" style="3" customWidth="1"/>
-    <col min="15" max="18" width="57.28515625" style="3" customWidth="1"/>
+    <col min="11" max="12" width="45.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" style="3" customWidth="1"/>
+    <col min="15" max="18" width="39.140625" style="3" customWidth="1"/>
     <col min="19" max="21" width="42.85546875" style="3" customWidth="1"/>
-    <col min="22" max="22" width="84.28515625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="34.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>645</v>
+        <v>2</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>7</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>5</v>
+        <v>450</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>620</v>
+      <c r="N1" s="16" t="s">
+        <v>7</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P1" s="16" t="s">
         <v>627</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="R1" s="16" t="s">
         <v>628</v>
       </c>
       <c r="S1" s="16" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="T1" s="16" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="U1" s="16" t="s">
-        <v>459</v>
-      </c>
-      <c r="V1" s="16" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="409.5" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>641</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>641</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>644</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>646</v>
+      </c>
+      <c r="P2" s="22" t="s">
+        <v>647</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>649</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>651</v>
+      </c>
+      <c r="T2" s="22" t="s">
+        <v>650</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="V2" s="22" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>638</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="O3" s="22" t="s">
         <v>636</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>630</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>637</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>644</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>652</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>647</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="Q3" s="22" t="s">
         <v>648</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>652</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>646</v>
+        <v>630</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>631</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>649</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -3403,29 +3377,17 @@
           </x14:formula1>
           <xm:sqref>G1</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'CV values'!$D$2:$D$60</xm:f>
-          </x14:formula1>
-          <xm:sqref>F3:F1048576</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K1</xm:sqref>
+          <xm:sqref>K1:L1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
           <xm:sqref>S1:U1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>V1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -3438,6 +3400,18 @@
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
           <xm:sqref>O1:R1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
+          <x14:formula1>
+            <xm:f>'CV values'!$B$2:$B$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list">
+          <x14:formula1>
+            <xm:f>'CV values'!$D$2:$D$60</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3465,31 +3439,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3497,2059 +3471,2059 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>490</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>507</v>
+        <v>491</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>508</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>624</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>453</v>
-      </c>
-      <c r="G7" s="21" t="s">
+        <v>454</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>621</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>532</v>
-      </c>
-      <c r="E9" s="18" t="s">
+        <v>533</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>626</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>534</v>
-      </c>
-      <c r="E11" s="18" t="s">
+        <v>535</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>627</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>629</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="20" t="s">
         <v>622</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="20" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>542</v>
-      </c>
-      <c r="E29" s="18" t="s">
+        <v>543</v>
+      </c>
+      <c r="E29" s="17" t="s">
         <v>625</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>545</v>
-      </c>
-      <c r="E36" s="20"/>
+        <v>546</v>
+      </c>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E37" s="18"/>
+        <v>111</v>
+      </c>
+      <c r="E37" s="17"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>546</v>
-      </c>
-      <c r="E38" s="19"/>
+        <v>547</v>
+      </c>
+      <c r="E38" s="18"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="14" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="14" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="14" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="14" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="14" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="14" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="14" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="14" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="14" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="14" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="14" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" s="14" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C123" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" s="14" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" s="14" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C125" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" s="14" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C126" s="10" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" s="14" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="14" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C129" s="10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="14" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C130" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="14" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="14" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C132" s="10" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C133" s="10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C134" s="10" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="14" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="14" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="14" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="14" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C140" s="10" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" s="14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C141" s="14" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" s="14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C142" s="14" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="14" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C143" s="14" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="14" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C144" s="14" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" s="14" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C146" s="10" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" s="14" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C147" s="10" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" s="14" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C148" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" s="14" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C149" s="14" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" s="14" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C150" s="14" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" s="14" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C151" s="14" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="14" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" s="14" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" s="14" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C154" s="14" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" s="14" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" s="14" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C156" s="10" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" s="14" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" s="14" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C158" s="10" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" s="14" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" s="14" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" s="14" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" s="14" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C163" s="14" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" s="14" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C164" s="14" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" s="14" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C165" s="14" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" s="14" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C166" s="14" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" s="14" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C167" s="14" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" s="14" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C168" s="14" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" s="14" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C169" s="14" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" s="14" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C170" s="14" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" s="14" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C171" s="14" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" s="14" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C172" s="14" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" s="14" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" s="14" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" s="14" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C175" s="14" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" s="14" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C176" s="14" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" s="14" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C177" s="14" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" s="14" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C178" s="14" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" s="14" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C179" s="14" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" s="14" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C180" s="14" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" s="14" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C181" s="14" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" s="14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" s="14" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" s="14" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C184" s="14" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" s="14" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C185" s="14" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" s="14" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C186"/>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" s="14" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C187"/>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" s="14" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C188"/>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" s="14" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C189"/>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" s="14" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C190"/>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" s="14" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C191"/>
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" s="14" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C192"/>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" s="14" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C193"/>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C194"/>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" s="14" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C195"/>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" s="14" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C196"/>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" s="14" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C197"/>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" s="14" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C198"/>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" s="14" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C199"/>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" s="14" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C200"/>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" s="14" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C201"/>
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" s="14" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C202"/>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" s="14" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C203"/>
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" s="14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C204"/>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" s="14" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C205"/>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" s="14" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C206"/>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" s="14" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C207"/>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" s="14" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C208"/>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" s="14" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C209"/>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" s="14" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C210"/>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" s="14" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C211"/>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" s="14" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C212"/>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" s="14" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C213"/>
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214" s="14" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C214"/>
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" s="14" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C215"/>
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" s="14" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C216"/>
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217" s="14" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C217"/>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" s="14" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C218"/>
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" s="14" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C219"/>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" s="14" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C220"/>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" s="14" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C221"/>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" s="14" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C222"/>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" s="14" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C223"/>
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" s="14" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C224"/>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225" s="14" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C225"/>
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" s="14" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C226"/>
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227" s="14" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C227"/>
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228" s="14" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C228"/>
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B229" s="14" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C229"/>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230" s="14" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C230"/>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231" s="14" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C231"/>
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" s="14" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C232"/>
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233" s="14" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C233"/>
     </row>
@@ -5883,437 +5857,437 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>357</v>
-      </c>
       <c r="E2" s="7" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>362</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>375</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>365</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>369</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>372</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>473</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>374</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>377</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>380</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>383</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>386</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>394</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>396</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>398</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>400</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>402</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>404</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D23" s="7" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D24" s="7" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D25" s="7" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D26" s="7" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D27" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D28" s="7" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D29" s="7" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D30" s="7" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D31" s="7" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D32" s="7" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="7" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="7" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="7" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="7" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="7" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="7" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="7" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="7" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="7" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="7" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="7" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="7" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="7" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="7" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="7" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="7" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="7" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="7" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="7" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="7" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="7" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>